<commit_message>
detalles arreglado y crear falta arreglar
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\EjemploProyecto\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9CFEF1-5349-4D79-B38C-53255D1774EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01237160-3FFD-4057-A2EE-C1F7748A2E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Alumno</t>
   </si>
@@ -40,13 +40,16 @@
   </si>
   <si>
     <t>Creacion proyecto, funciones listar y detalles</t>
+  </si>
+  <si>
+    <t>Detalles arreglado, creación medio hecho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +61,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,15 +97,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -367,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D2"/>
+  <dimension ref="B1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,6 +420,17 @@
         <v>45765</v>
       </c>
     </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45765</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
eliminar: proyecto, tarea, empleado
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\EjemploProyecto\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01237160-3FFD-4057-A2EE-C1F7748A2E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24495E5-1381-4ACC-8EF0-5C2A67E2F7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Alumno</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Detalles arreglado, creación medio hecho</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Eliminar con botón desde detalles: Proyecto, Tarea, Empleado</t>
+  </si>
+  <si>
+    <t>Crear con forularios: Proyecto, Tarea, Empleado</t>
   </si>
 </sst>
 </file>
@@ -387,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D3"/>
+  <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,6 +440,28 @@
         <v>45765</v>
       </c>
     </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45767</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update hecho, hay que mejorar los enlaces
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\EjemploProyecto\ProyectoWeb2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24495E5-1381-4ACC-8EF0-5C2A67E2F7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0530801D-9609-4C87-BD33-E6810561D247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Alumno</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Crear con forularios: Proyecto, Tarea, Empleado</t>
+  </si>
+  <si>
+    <t>Update hecho</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D5"/>
+  <dimension ref="B1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,6 +465,17 @@
         <v>45767</v>
       </c>
     </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45767</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ultimos mpleados en footer
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2728F772-0B42-47F7-B9EC-93757BCA34ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6E06DC-FCDC-49E8-A180-8446975238B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4755" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Alumno</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Modelo tarea arreglado</t>
+  </si>
+  <si>
+    <t>Footer con últimos empleados (extra)</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D8"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +507,17 @@
         <v>45772</v>
       </c>
     </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45773</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
footer con ultimos 3 del modelo correspondiente
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6E06DC-FCDC-49E8-A180-8446975238B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32765925-9987-4D06-8718-C1399D3BFA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4755" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>Modelo tarea arreglado</t>
   </si>
   <si>
-    <t>Footer con últimos empleados (extra)</t>
+    <t>Footer con últimos empleados, herramientas, tareas, empleados (extra)</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +515,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="2">
-        <v>45773</v>
+        <v>45774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
segunda linea de menu horizontal, botón de editar
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32765925-9987-4D06-8718-C1399D3BFA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA7CCD4-8685-4A4D-BAED-5609AB5A4489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4755" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Alumno</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Footer con últimos empleados, herramientas, tareas, empleados (extra)</t>
+  </si>
+  <si>
+    <t>Segunda linea de menu horizontal, botón de editar en los detalles</t>
   </si>
 </sst>
 </file>
@@ -408,15 +411,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D9"/>
+  <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="68.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
@@ -518,6 +522,17 @@
         <v>45774</v>
       </c>
     </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2">
+        <v>45776</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ultimos tres en body y estilos de formulario arreglados
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA7CCD4-8685-4A4D-BAED-5609AB5A4489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B6D9A6-F30C-42C8-8F6D-E8C48BD4E32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Alumno</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Segunda linea de menu horizontal, botón de editar en los detalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultimos tres en body, estilos de crear </t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D10"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +536,17 @@
         <v>45776</v>
       </c>
     </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45778</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tareas en proceso del listado de tareas
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B6D9A6-F30C-42C8-8F6D-E8C48BD4E32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409DD941-19B3-43BA-B79E-ABA9F12DAF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Alumno</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ultimos tres en body, estilos de crear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tareas en proceso del listado </t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D11"/>
+  <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,6 +550,17 @@
         <v>45778</v>
       </c>
     </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45780</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Extras: Herramientas con baja disponibilidad y proyectos con alto presupuesto
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409DD941-19B3-43BA-B79E-ABA9F12DAF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44F66D7-4A51-4EAA-9907-EF3BA0B77AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Alumno</t>
   </si>
@@ -72,13 +72,22 @@
     <t xml:space="preserve">Ultimos tres en body, estilos de crear </t>
   </si>
   <si>
-    <t xml:space="preserve">Tareas en proceso del listado </t>
+    <t>Extra: Tareas "en proceso" del listado de tareas</t>
+  </si>
+  <si>
+    <t>Extra: Herramientas con baja disponibilidad del listado de herramientas</t>
+  </si>
+  <si>
+    <t>Extra: Proyectos de alto presupuesto del listado de proyectos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-C0A]d\-mmm;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,11 +140,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -417,16 +427,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D12"/>
+  <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="68.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
@@ -561,7 +571,30 @@
         <v>45780</v>
       </c>
     </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4">
+        <v>45782</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
subo el extra anotado en el excel
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44F66D7-4A51-4EAA-9907-EF3BA0B77AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270D290D-5F0F-4140-9F41-683E9D9B8C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Alumno</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Extra: Proyectos de alto presupuesto del listado de proyectos</t>
+  </si>
+  <si>
+    <t>Extra: Empleados no disponibles del listado de empleados</t>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-C0A]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-C0A]d\-mmm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -145,7 +148,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D14"/>
+  <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +596,17 @@
         <v>45782</v>
       </c>
     </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45783</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correccion de errores, nombres y etiquetas de codigo. Estilo ultimos registros y ajustes de css.
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\E2_IW_2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270D290D-5F0F-4140-9F41-683E9D9B8C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519E21E0-170D-44F1-8E01-DE74EE30BF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>Alumno</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Extra: Empleados no disponibles del listado de empleados</t>
+  </si>
+  <si>
+    <t>Estilos: Base, Create y Formularios</t>
+  </si>
+  <si>
+    <t>Estilos: Detalles de proyectos, empleados y tareas</t>
+  </si>
+  <si>
+    <t>Estilos: Logos footer</t>
+  </si>
+  <si>
+    <t>Estilos: Ultimos empleados, proyectos, tareas y herramientas</t>
+  </si>
+  <si>
+    <t>Boton eliminar y editar en "Detalles"</t>
+  </si>
+  <si>
+    <t>Correccion y limpieza en codigo</t>
   </si>
 </sst>
 </file>
@@ -430,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D15"/>
+  <dimension ref="B1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,10 +506,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2">
         <v>45767</v>
@@ -513,21 +531,21 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2">
-        <v>45771</v>
+        <v>45767</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2">
-        <v>45772</v>
+        <v>45770</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -535,10 +553,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2">
-        <v>45774</v>
+        <v>45771</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -546,10 +564,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2">
-        <v>45776</v>
+        <v>45772</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -557,21 +575,21 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2">
-        <v>45778</v>
+        <v>45774</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2">
-        <v>45780</v>
+        <v>45775</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -579,10 +597,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="4">
-        <v>45782</v>
+        <v>13</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45776</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -590,20 +608,86 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="4">
-        <v>45782</v>
+        <v>14</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45778</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="2">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45780</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="4">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="4">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D20" s="2">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="2">
         <v>45783</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Última subida, damos por finalizada la entrega
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\proyectoColaborativo\ProyectoWeb2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13903979-EB8F-4F81-A66F-BFA4AC912EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E410E2A0-85E1-41E9-907F-6D2479AFFD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Alumno</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Tarea</t>
   </si>
   <si>
-    <t>Fecha</t>
-  </si>
-  <si>
     <t>Gaizka</t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>Actualización de los registros de la BD</t>
+  </si>
+  <si>
+    <t>Fecha fin e inicio</t>
+  </si>
+  <si>
+    <t>Mostrar las herramientas por tarea (many to many)</t>
   </si>
 </sst>
 </file>
@@ -484,19 +487,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F30"/>
+  <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="68.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,326 +507,337 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="2">
         <v>45765</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2">
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2">
         <v>45767</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
         <v>45767</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2">
         <v>45767</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2">
         <v>45770</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2">
         <v>45772</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
       </c>
       <c r="D10" s="2">
         <v>45772</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2">
         <v>45771</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2">
         <v>45772</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2">
         <v>45774</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2">
         <v>45775</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2">
         <v>45776</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2">
         <v>45776</v>
       </c>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2">
         <v>45776</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2">
         <v>45777</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2">
         <v>45777</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2">
         <v>45778</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="2">
         <v>45779</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="2">
         <v>45779</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="2">
         <v>45780</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2">
         <v>45781</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="4">
         <v>45782</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" s="4">
         <v>45782</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="4">
         <v>45782</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="2">
         <v>45783</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D29" s="2">
         <v>45783</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="2">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="2">
         <v>45784</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ultima subida del proyecto, damos por finalizada la entrega
</commit_message>
<xml_diff>
--- a/organizacion.xlsx
+++ b/organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E410E2A0-85E1-41E9-907F-6D2479AFFD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6897D418-433F-4396-8CCB-73D77FB5BC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Alumno</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Mostrar las herramientas por tarea (many to many)</t>
+  </si>
+  <si>
+    <t>Esquema entidad relación</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F31"/>
+  <dimension ref="B1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,6 +844,17 @@
         <v>45784</v>
       </c>
     </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="2">
+        <v>45784</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>